<commit_message>
Biblio for discussion, conclusion
</commit_message>
<xml_diff>
--- a/Biblio/Biblio_16122024.xlsx
+++ b/Biblio/Biblio_16122024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP2\Desktop\Methodo_stat_donnees\Biblio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6D081E-1277-4386-BD21-E3EAD57AF651}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC86E910-CDB3-4F11-8514-E10E0F8DFE14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="3620" xr2:uid="{5F726666-A13F-427B-B1DF-EF1B7AF8E8BC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="377">
   <si>
     <t>Reference</t>
   </si>
@@ -1099,6 +1099,99 @@
   </si>
   <si>
     <t>Gaussian mixture modeling = non-supervised clustering-like process; able to identify the 8 most characteristic types of patient adherence behavior. Step 1: detecting summarization patterns using the Matrix Profile method (=2 time series to be similar if they share many similar subsequences, regardless of the order and time of matching). Step 2: features extraction and selection; to build sets of snippets in which the elements carried common characteristics so to determine the most common 30-day behaviors of patients using TSFE library. Step 3: selection; PCA with BIC. GMM = probalistic technique for representing normally distributed subpopulations that pertain to a bigger statset; estimation obtained with an iterative EM process that seeks a maximum likelihood estimation over a given number of components; each components is described by its mean and variance and we obtained a probability. The optimal number of distribution components was defined using the BIC. CAn use also Log-likelihood, AIC, AWE, Consistent AIC, Kullback information Criterion (KIC), Sample size-adjusted BIC and ICL (Integrated Completed Likelihood). Visualisation of the components via GMM using linear discriminant analysis (LDA): project the CPAP use dataset onto a 3D space; LDA similar to PCA finds the component axes that maximize the variance of the data at the same time that it sets axes to maximize the separation between classes.</t>
+  </si>
+  <si>
+    <t>Clustering algorithms: a comparative approach, Plos One</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0210236</t>
+  </si>
+  <si>
+    <t>9 clustering methods: EM, clara, k-means, hcmodel, hierarchical, spectral, optics, dbscan</t>
+  </si>
+  <si>
+    <t>400 artificial datasets</t>
+  </si>
+  <si>
+    <t>Spectral method provides the best performance when using default parameters / not significant for low-dimensional datasets regarding the default parameters / underestimating the number of classes in the dataset led to worse performance than in overestimation situations for all algorithms.                                                                                           Regarding single parameter variations, hierarchical, optics and EM methods significant performance variation.                             Algorithms are not sensitive to parameter variations for this dataset (10 classes and 2 features) / 2 classes and 10 features: EM, hcmodel, subspace and iherarchical algo significant gain in performance</t>
+  </si>
+  <si>
+    <t>Performance evaluation of distance metrics in the clustering algorithms, INFOCOMP</t>
+  </si>
+  <si>
+    <t>Mayra Z. Rodriguez, 2019</t>
+  </si>
+  <si>
+    <t>v. 13, no. 1, p. 38-51</t>
+  </si>
+  <si>
+    <t>Vijay Kumar, 2014</t>
+  </si>
+  <si>
+    <t>Hierarchical techniques, partitional clustering techniques with different measures: euclidean, standardized euclidean, Manhattan distance, Mahalanbois distance, Cosine disctance, Correlation distance, Spearman disctance, Cheybyshev distance, Canberra distance, Bray-Curtis distance</t>
+  </si>
+  <si>
+    <t>3 artificial and 6 real-life datasets</t>
+  </si>
+  <si>
+    <t>There is no single best distance measure for all datasets or for all quality measures. The appropriateness of a distance measure is dependent on nature of data and clustering technique.                                                                                  Hierarchical techniques: single linkage, average linkage, complete linkage, weighted linkage / Partitional techinques: K-means, K-medoid, ACOC, MHSC</t>
+  </si>
+  <si>
+    <t>Comparison of clustering techniques for cluster analysis, Nat Sci</t>
+  </si>
+  <si>
+    <t>43 : 378 - 388</t>
+  </si>
+  <si>
+    <t>Piyatida Rujasiri and Boonorm Chomtee, 2009</t>
+  </si>
+  <si>
+    <t>Hierarchical, K-means, SOM, K-medoids and K-medoids integrated with DTW</t>
+  </si>
+  <si>
+    <t>Simulated and real datasets</t>
+  </si>
+  <si>
+    <t>K-means and Kohonen's SOM yielded the lowest RMSSTD ans highest RS for the 3, 5 and 7 variables and for 2, 3, 4, 5, 6, 7 and 8 custers / increasing the number of clusters tended to increase the efficiency of the 5 clustering methods / number of variables did not affect the efficiency of the 5 clustering methods, which indicated that K-meabs and SOM were the most suitable algo / clustering the real dataset produced the same results with both the study and the simulated data.</t>
+  </si>
+  <si>
+    <t>10.3233/IDA-2007-11602</t>
+  </si>
+  <si>
+    <t>An overview of clustering methods, Intelligent Data Analysis</t>
+  </si>
+  <si>
+    <t>Mahamed G.H. Omran, 2014</t>
+  </si>
+  <si>
+    <t>Hierarchical Clustering Techniques, Partitional Clustering Techniques: K-means algo, Fuzzy C-means algo, Gaussian EM algo, K-harmonic Means algo, Hybrid 2, non-iterative Partitional algo, Other clustering techniques as Nearest Neighbor, Spectral, SOM, Stochastic algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data clustering problem definition / Terms definition / Overview of the different similarity measures / Clustering techniques discussed / Presentation of different clustering validation techniques / Methods that automatically determine the number of clusters in a data set / Overview of clustering using SOMs and stochastic techniques </t>
+  </si>
+  <si>
+    <t>Bayesian kernel machine regression-causal mediation analysis, Stat Med</t>
+  </si>
+  <si>
+    <t>10.1002/sim.9255.</t>
+  </si>
+  <si>
+    <t>Katrina L. Devick</t>
+  </si>
+  <si>
+    <t>BKMR</t>
+  </si>
+  <si>
+    <t>New methodology to estimate natural direct and indirect effects and controlled direct effects of a complex mixture exposure on an outcome through a mediator variable / when the exposure-mediator and exposure-mediator-outcome relationships are complex, BKMR-Causal mediation analysis performs better than current mediation methods</t>
+  </si>
+  <si>
+    <t>children's neurodevelopmental scores</t>
+  </si>
+  <si>
+    <t>in utero co-exposure to arsenic, manganese and lead + birth lengths as a mediator</t>
+  </si>
+  <si>
+    <t>Simulation study &amp; real life data (prospective birth cohort in Bangladesh)</t>
   </si>
 </sst>
 </file>
@@ -1580,11 +1673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62570392-9DE9-466D-863E-48ADE7AB8533}">
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2766,6 +2859,109 @@
         <v>345</v>
       </c>
     </row>
+    <row r="49" spans="1:11" s="4" customFormat="1" ht="174" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A51" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{A4FCDD30-7E2C-471D-9F4C-391A5B5ACC7C}"/>
@@ -2786,9 +2982,10 @@
     <hyperlink ref="B43" r:id="rId16" xr:uid="{85E7914D-D8DB-4D85-B59E-67380AB17AE3}"/>
     <hyperlink ref="B47" r:id="rId17" xr:uid="{D6E4518F-2ECA-4F56-904E-6577D01115B8}"/>
     <hyperlink ref="B48" r:id="rId18" xr:uid="{74B127ED-5E0A-4C22-A4EE-57FFA1C76579}"/>
+    <hyperlink ref="B49" r:id="rId19" xr:uid="{B192C44F-88A1-4889-B5FC-D2FABCF11A5F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GMM ARIMA RICLPM HMM and survival methods changed
</commit_message>
<xml_diff>
--- a/Biblio/Biblio_16122024.xlsx
+++ b/Biblio/Biblio_16122024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP2\Desktop\Methodo_stat_donnees\Biblio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BF1686-F3D1-436A-AA5D-28466B75507E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC297A7-E486-4768-A6B2-B488BCE5EA76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="3620" xr2:uid="{5F726666-A13F-427B-B1DF-EF1B7AF8E8BC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="398">
   <si>
     <t>Reference</t>
   </si>
@@ -1240,6 +1240,21 @@
   </si>
   <si>
     <t>RI-CLPM in wide-format using structural equation modeling (SEM). To fit an RI-CLPM we need to decompose the observed scores into 3 components: grand means, stable between components and fluctuating within components. First, the grand means may be time-varying or may be fixed to be invariant over time. Second, the between components capture a unit's time-invariant deviation from the grand means and thus represent the stable differences between units. The random intercepts are specified in SEM software by creating a latent variable with the repeated measures as its indicators and fixing all the factor loadings to 1. Third, the within components are the differences between a units observed measurements and the unit's expected score based on the grand means and its random intercepts: create them in SEM software by specifying a latent variable for each measurement and constraining its measurement error variances to 0; next specify the structural relations between the within components; the autoregressive effects represent the within-person carry-over effects (sometimes the within-person autoregressive effects are referred to as inertia (the tendency to not move)); the cross-lagged effects in the model represent the spill-over of the state in 1 domain into the state of another domain. Ability to test specific hypotheses imposing constraints on the model and test the tenability of these constraints or AIC, BIC as measures of model fit to compare both non-nested and nested models, the use of chi² difference test is wide-spread in the SEM community but a few cautionary notes are in order. To fit a model with freely estimated factor loadings, at least 4 occasions of data are needed; in contrast with the fixed factor loadings, the model is already identified with lony 3 waves of data. Extensions of teh basis RI-CLPM: including time-invariant predictors and outcomes, the multi group RI-CLPM, the multiple indicator RI-CLPM</t>
+  </si>
+  <si>
+    <t>A critique of the Random Intercept Cross-Lagged Panel Model, PsyArXiv</t>
+  </si>
+  <si>
+    <t>doi: 10.31234/osf.io/6f85c</t>
+  </si>
+  <si>
+    <t>Olivier Lüdtke and Alexander Robitzsch, 2021</t>
+  </si>
+  <si>
+    <t>RI-CLPM / CLPM (Formal analysis and simulated data)</t>
+  </si>
+  <si>
+    <t>RI-CLPM = extension of CLPM that allows controlling for stable trait factors when estimating cross-lagged effects. RI-CLPM more appropriately accounts for trait-like, time-invariant stability of many psychological constructs, preferred to CLPM when at least 3 waves of measurements are available.                                                                                                        Only a limited potential to adjust for unobserved confounding estimates of teh cross-lagged effect will generaly be biased unless very restrictive condition for the effects of the confounder variable are met.                                                                                                                                                                                                               If the main goal is to assess the potential effects of causes that makes persons differences from other persons - and not from the long-term average lvel - the CLPM should be preferred. =&gt; RICLPM better suited for short-term studies of states using shorter time lags (e.g. days) between 2 assessment and are not concerned about systematic long term changes.</t>
   </si>
 </sst>
 </file>
@@ -1357,7 +1372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1405,6 +1420,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1721,11 +1739,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62570392-9DE9-466D-863E-48ADE7AB8533}">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3060,6 +3078,26 @@
       </c>
       <c r="K55" s="4" t="s">
         <v>392</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="K56" s="15" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>